<commit_message>
sepration of test and train file
</commit_message>
<xml_diff>
--- a/app/data/fish/DAIMON_Cod_Data_FDI_TEST.xlsx
+++ b/app/data/fish/DAIMON_Cod_Data_FDI_TEST.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="203">
   <si>
     <t>project</t>
   </si>
@@ -265,73 +265,373 @@
     <t>DAIMON</t>
   </si>
   <si>
-    <t>WH0408/B13/1/2/LEEXT</t>
+    <t>WH0408/B09/7/11/LEEXT</t>
   </si>
   <si>
     <t>WH0408</t>
   </si>
   <si>
+    <t>B09</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>LEEXT</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>1.64</t>
+  </si>
+  <si>
+    <t>6.38</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>HistoRoutine (TI-FI)</t>
+  </si>
+  <si>
+    <t>4541 - HK 49</t>
+  </si>
+  <si>
+    <t>WH0408/B09/8/6/EXT</t>
+  </si>
+  <si>
+    <t>EXT</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>WH0408/B09/8/5/EXT</t>
+  </si>
+  <si>
+    <t>WH0408/B09/8/4/EXT</t>
+  </si>
+  <si>
+    <t>WH0408/B09/8/3/LEEXT</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>WH0408/B09/7/12/LEEXT</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>1.68</t>
+  </si>
+  <si>
+    <t>6.49</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>4544 - HK 50</t>
+  </si>
+  <si>
+    <t>WH0408/B09/8/19/LEEXT</t>
+  </si>
+  <si>
+    <t>WH0401/B13/14/3/LEEXT</t>
+  </si>
+  <si>
+    <t>WH0401</t>
+  </si>
+  <si>
     <t>B13</t>
   </si>
   <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>LEEXT</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1.49</t>
-  </si>
-  <si>
-    <t>5.99</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>HistoRoutine (TI-FI)</t>
-  </si>
-  <si>
-    <t>4207 - HK 2</t>
-  </si>
-  <si>
-    <t>WH0408/B13/1/3/LEEXT</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1.38</t>
-  </si>
-  <si>
-    <t>5.49</t>
-  </si>
-  <si>
-    <t>0.7</t>
+    <t>M 120</t>
+  </si>
+  <si>
+    <t>S 120</t>
+  </si>
+  <si>
+    <t>MU 120</t>
+  </si>
+  <si>
+    <t>B 115</t>
+  </si>
+  <si>
+    <t>V 120</t>
+  </si>
+  <si>
+    <t>FOE 91</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>5.8</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>4209 - HK 3</t>
+    <t>BH 91</t>
+  </si>
+  <si>
+    <t>BP 91</t>
+  </si>
+  <si>
+    <t>L 120</t>
+  </si>
+  <si>
+    <t>H 120</t>
+  </si>
+  <si>
+    <t>K 120</t>
+  </si>
+  <si>
+    <t>Oto 120</t>
+  </si>
+  <si>
+    <t>WH0401/B13/14/2/LEEXT</t>
+  </si>
+  <si>
+    <t>M 119</t>
+  </si>
+  <si>
+    <t>S 119</t>
+  </si>
+  <si>
+    <t>MU 119</t>
+  </si>
+  <si>
+    <t>B 114</t>
+  </si>
+  <si>
+    <t>V 119</t>
+  </si>
+  <si>
+    <t>U 21</t>
+  </si>
+  <si>
+    <t>FOE 90</t>
+  </si>
+  <si>
+    <t>1.91</t>
+  </si>
+  <si>
+    <t>7.56</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>36.5</t>
+  </si>
+  <si>
+    <t>BH 90</t>
+  </si>
+  <si>
+    <t>BP 90</t>
+  </si>
+  <si>
+    <t>L 119</t>
+  </si>
+  <si>
+    <t>H 119</t>
+  </si>
+  <si>
+    <t>K 119</t>
+  </si>
+  <si>
+    <t>Oto 119</t>
+  </si>
+  <si>
+    <t>WH0401/B13/14/1/LEEXT</t>
+  </si>
+  <si>
+    <t>M 118</t>
+  </si>
+  <si>
+    <t>S 118</t>
+  </si>
+  <si>
+    <t>MU 118</t>
+  </si>
+  <si>
+    <t>B 113</t>
+  </si>
+  <si>
+    <t>V 118</t>
+  </si>
+  <si>
+    <t>U 20</t>
+  </si>
+  <si>
+    <t>FOE 89</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>6.11</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>BH 89</t>
+  </si>
+  <si>
+    <t>BP 89</t>
+  </si>
+  <si>
+    <t>L 118</t>
+  </si>
+  <si>
+    <t>H 118</t>
+  </si>
+  <si>
+    <t>K 118</t>
+  </si>
+  <si>
+    <t>Oto 118</t>
+  </si>
+  <si>
+    <t>WH0401/B13/13/2/LEEXT</t>
+  </si>
+  <si>
+    <t>M 117</t>
+  </si>
+  <si>
+    <t>S 117</t>
+  </si>
+  <si>
+    <t>MU 117</t>
+  </si>
+  <si>
+    <t>B 112</t>
+  </si>
+  <si>
+    <t>V 117</t>
+  </si>
+  <si>
+    <t>FOE 88</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>29.5</t>
+  </si>
+  <si>
+    <t>BH 88</t>
+  </si>
+  <si>
+    <t>BP 88</t>
+  </si>
+  <si>
+    <t>L 117</t>
+  </si>
+  <si>
+    <t>H 117</t>
+  </si>
+  <si>
+    <t>K 117</t>
+  </si>
+  <si>
+    <t>HK_RTE 3700</t>
+  </si>
+  <si>
+    <t>Oto 117</t>
+  </si>
+  <si>
+    <t>WH0401/B13/13/1/LEEXT</t>
+  </si>
+  <si>
+    <t>M 116</t>
+  </si>
+  <si>
+    <t>S 116</t>
+  </si>
+  <si>
+    <t>MU 116</t>
+  </si>
+  <si>
+    <t>B 111</t>
+  </si>
+  <si>
+    <t>V 116</t>
+  </si>
+  <si>
+    <t>FOE 87</t>
+  </si>
+  <si>
+    <t>2.01</t>
+  </si>
+  <si>
+    <t>7.66</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>BH 87</t>
+  </si>
+  <si>
+    <t>BP 87</t>
+  </si>
+  <si>
+    <t>L 116</t>
+  </si>
+  <si>
+    <t>H 116</t>
+  </si>
+  <si>
+    <t>K 116</t>
+  </si>
+  <si>
+    <t>Oto 116</t>
   </si>
 </sst>
 </file>
@@ -728,7 +1028,7 @@
   <dimension ref="A1:CQ1426"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="A9" sqref="A9:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,7 +1363,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>81</v>
@@ -1075,7 +1375,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>82</v>
@@ -1087,37 +1387,37 @@
         <v>84</v>
       </c>
       <c r="L2" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>85</v>
       </c>
       <c r="N2" s="2">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="O2" s="2">
-        <v>394</v>
+        <v>1133</v>
       </c>
       <c r="P2" s="2">
-        <v>55.358499999999999</v>
+        <v>55.244</v>
       </c>
       <c r="Q2" s="2">
-        <v>15.54933333</v>
+        <v>18.166333330000001</v>
       </c>
       <c r="R2" s="2">
-        <v>6.97</v>
+        <v>6.98</v>
       </c>
       <c r="S2" s="2">
-        <v>18.010000000000002</v>
+        <v>17.91</v>
       </c>
       <c r="T2" s="2">
-        <v>11.41</v>
+        <v>11.75</v>
       </c>
       <c r="U2" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V2" s="2">
-        <v>-0.184</v>
+        <v>11.2715</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>86</v>
@@ -1168,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="AM2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN2" s="2">
         <v>0</v>
       </c>
       <c r="AO2" s="2">
-        <v>0.71803469900000005</v>
+        <v>0.90639999999999998</v>
       </c>
       <c r="AP2" s="5" t="s">
         <v>87</v>
@@ -1190,46 +1490,44 @@
         <v>88</v>
       </c>
       <c r="BC2" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="BE2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="BF2" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="BF2" s="5"/>
       <c r="BG2" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="BH2" s="2" t="s">
         <v>88</v>
       </c>
       <c r="BI2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BJ2" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="BK2" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="BL2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BN2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="BP2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BQ2" s="2" t="s">
         <v>88</v>
@@ -1247,17 +1545,15 @@
         <v>88</v>
       </c>
       <c r="BV2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BX2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BY2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="BZ2" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="BZ2" s="5"/>
       <c r="CA2" s="2" t="s">
         <v>88</v>
       </c>
@@ -1283,10 +1579,10 @@
         <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>81</v>
@@ -1298,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="H3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>82</v>
@@ -1307,323 +1603,1780 @@
         <v>83</v>
       </c>
       <c r="K3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>48</v>
+      </c>
+      <c r="O3">
+        <v>871</v>
+      </c>
+      <c r="P3">
+        <v>55.240666670000003</v>
+      </c>
+      <c r="Q3">
+        <v>18.170333329999998</v>
+      </c>
+      <c r="R3">
+        <v>6.96</v>
+      </c>
+      <c r="S3">
+        <v>17.97</v>
+      </c>
+      <c r="T3">
+        <v>11.73</v>
+      </c>
+      <c r="U3">
+        <v>88</v>
+      </c>
+      <c r="V3">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0.78757957199999995</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>2017</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4">
+        <v>37</v>
+      </c>
+      <c r="O4">
+        <v>540</v>
+      </c>
+      <c r="P4">
+        <v>55.240666670000003</v>
+      </c>
+      <c r="Q4">
+        <v>18.170333329999998</v>
+      </c>
+      <c r="R4">
+        <v>6.96</v>
+      </c>
+      <c r="S4">
+        <v>17.97</v>
+      </c>
+      <c r="T4">
+        <v>11.73</v>
+      </c>
+      <c r="U4">
+        <v>88</v>
+      </c>
+      <c r="V4">
+        <v>-0.184</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>1.0660770340000001</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5">
+        <v>2017</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>46</v>
+      </c>
+      <c r="O5">
+        <v>826</v>
+      </c>
+      <c r="P5">
+        <v>55.240666670000003</v>
+      </c>
+      <c r="Q5">
+        <v>18.170333329999998</v>
+      </c>
+      <c r="R5">
+        <v>6.96</v>
+      </c>
+      <c r="S5">
+        <v>17.97</v>
+      </c>
+      <c r="T5">
+        <v>11.73</v>
+      </c>
+      <c r="U5">
+        <v>88</v>
+      </c>
+      <c r="V5">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0.84860688699999998</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6">
+        <v>2017</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
         <v>84</v>
       </c>
-      <c r="L3">
+      <c r="L6">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6">
+        <v>48</v>
+      </c>
+      <c r="O6">
+        <v>1086</v>
+      </c>
+      <c r="P6">
+        <v>55.240666670000003</v>
+      </c>
+      <c r="Q6">
+        <v>18.170333329999998</v>
+      </c>
+      <c r="R6">
+        <v>6.96</v>
+      </c>
+      <c r="S6">
+        <v>17.97</v>
+      </c>
+      <c r="T6">
+        <v>11.73</v>
+      </c>
+      <c r="U6">
+        <v>88</v>
+      </c>
+      <c r="V6">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0.98198784699999997</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7">
+        <v>2017</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
         <v>85</v>
       </c>
-      <c r="N3">
-        <v>32</v>
-      </c>
-      <c r="O3">
-        <v>216</v>
-      </c>
-      <c r="P3">
-        <v>55.358499999999999</v>
-      </c>
-      <c r="Q3">
-        <v>15.54933333</v>
-      </c>
-      <c r="R3">
-        <v>6.97</v>
-      </c>
-      <c r="S3">
-        <v>18.010000000000002</v>
-      </c>
-      <c r="T3">
-        <v>11.41</v>
-      </c>
-      <c r="U3">
-        <v>90</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3" s="6" t="s">
+      <c r="N7">
+        <v>37</v>
+      </c>
+      <c r="O7">
+        <v>461</v>
+      </c>
+      <c r="P7">
+        <v>55.244</v>
+      </c>
+      <c r="Q7">
+        <v>18.166333330000001</v>
+      </c>
+      <c r="R7">
+        <v>6.98</v>
+      </c>
+      <c r="S7">
+        <v>17.91</v>
+      </c>
+      <c r="T7">
+        <v>11.75</v>
+      </c>
+      <c r="U7">
+        <v>87</v>
+      </c>
+      <c r="V7">
+        <v>-0.184</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0.91011391200000002</v>
+      </c>
+      <c r="AP7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>109</v>
+      </c>
+      <c r="BJ7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>110</v>
+      </c>
+      <c r="BL7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>111</v>
+      </c>
+      <c r="BN7" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0.65917968800000004</v>
-      </c>
-      <c r="AP3" s="6" t="s">
+      <c r="BO7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BP7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>96</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>113</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>106</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8">
+        <v>2017</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8">
+        <v>30</v>
+      </c>
+      <c r="O8">
+        <v>270</v>
+      </c>
+      <c r="P8">
+        <v>55.240666670000003</v>
+      </c>
+      <c r="Q8">
+        <v>18.170333329999998</v>
+      </c>
+      <c r="R8">
+        <v>6.96</v>
+      </c>
+      <c r="S8">
+        <v>17.97</v>
+      </c>
+      <c r="T8">
+        <v>11.73</v>
+      </c>
+      <c r="U8">
+        <v>88</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AZ3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BC3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>98</v>
-      </c>
-      <c r="BJ3" s="6" t="s">
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9">
+        <v>2016</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N9">
+        <v>41</v>
+      </c>
+      <c r="O9">
+        <v>581</v>
+      </c>
+      <c r="P9">
+        <v>55.312666669999999</v>
+      </c>
+      <c r="Q9">
+        <v>15.574666669999999</v>
+      </c>
+      <c r="R9">
+        <v>18.21</v>
+      </c>
+      <c r="S9">
+        <v>6.8</v>
+      </c>
+      <c r="T9">
+        <v>1.96</v>
+      </c>
+      <c r="U9">
+        <v>89</v>
+      </c>
+      <c r="V9">
+        <v>0.88270000000000004</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0.84299415300000002</v>
+      </c>
+      <c r="AP9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="BK3" t="s">
-        <v>99</v>
-      </c>
-      <c r="BL3" s="6" t="s">
+      <c r="AZ9" t="s">
+        <v>118</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>124</v>
+      </c>
+      <c r="BJ9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>126</v>
+      </c>
+      <c r="BN9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>127</v>
+      </c>
+      <c r="BP9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>129</v>
+      </c>
+      <c r="BS9" t="s">
+        <v>130</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>131</v>
+      </c>
+      <c r="BU9" t="s">
+        <v>132</v>
+      </c>
+      <c r="BV9" t="s">
+        <v>96</v>
+      </c>
+      <c r="CA9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10">
+        <v>2016</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10">
+        <v>40</v>
+      </c>
+      <c r="O10">
+        <v>510</v>
+      </c>
+      <c r="P10">
+        <v>55.312666669999999</v>
+      </c>
+      <c r="Q10">
+        <v>15.574666669999999</v>
+      </c>
+      <c r="R10">
+        <v>18.21</v>
+      </c>
+      <c r="S10">
+        <v>6.8</v>
+      </c>
+      <c r="T10">
+        <v>1.96</v>
+      </c>
+      <c r="U10">
+        <v>89</v>
+      </c>
+      <c r="V10">
+        <v>0.88270000000000004</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0.796875</v>
+      </c>
+      <c r="AP10" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="BM3" t="s">
-        <v>100</v>
-      </c>
-      <c r="BN3" s="6" t="s">
+      <c r="AZ10" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE10" t="s">
+        <v>139</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>143</v>
+      </c>
+      <c r="BL10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>144</v>
+      </c>
+      <c r="BN10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO10" t="s">
+        <v>145</v>
+      </c>
+      <c r="BP10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>146</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>147</v>
+      </c>
+      <c r="BS10" t="s">
+        <v>148</v>
+      </c>
+      <c r="BT10" t="s">
+        <v>149</v>
+      </c>
+      <c r="BU10" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV10" t="s">
+        <v>96</v>
+      </c>
+      <c r="CA10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11">
+        <v>2016</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11">
+        <v>36</v>
+      </c>
+      <c r="O11">
+        <v>457</v>
+      </c>
+      <c r="P11">
+        <v>55.312666669999999</v>
+      </c>
+      <c r="Q11">
+        <v>15.574666669999999</v>
+      </c>
+      <c r="R11">
+        <v>18.21</v>
+      </c>
+      <c r="S11">
+        <v>6.8</v>
+      </c>
+      <c r="T11">
+        <v>1.96</v>
+      </c>
+      <c r="U11">
+        <v>89</v>
+      </c>
+      <c r="V11">
+        <v>0.74829999999999997</v>
+      </c>
+      <c r="W11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="BO3" t="s">
-        <v>101</v>
-      </c>
-      <c r="BP3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>102</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="W6" s="5"/>
-      <c r="AP6" s="5"/>
-      <c r="AR6" s="5"/>
-      <c r="AZ6" s="3"/>
-      <c r="BA6" s="3"/>
-      <c r="BC6" s="5"/>
-      <c r="BF6" s="5"/>
-      <c r="BJ6" s="5"/>
-      <c r="BL6" s="5"/>
-      <c r="BN6" s="5"/>
-      <c r="BP6" s="5"/>
-      <c r="BZ6" s="5"/>
-      <c r="CB6" s="8"/>
-      <c r="CC6" s="8"/>
-      <c r="CD6" s="8"/>
-      <c r="CE6" s="8"/>
-      <c r="CF6" s="8"/>
-      <c r="CG6" s="8"/>
-      <c r="CH6" s="8"/>
-      <c r="CI6" s="8"/>
-      <c r="CJ6" s="8"/>
-      <c r="CK6" s="8"/>
-      <c r="CL6" s="8"/>
-      <c r="CM6" s="8"/>
-      <c r="CN6" s="8"/>
-      <c r="CO6" s="8"/>
-      <c r="CP6" s="8"/>
-      <c r="CQ6" s="8"/>
-    </row>
-    <row r="8" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="W8" s="5"/>
-      <c r="AP8" s="5"/>
-      <c r="AR8" s="5"/>
-      <c r="AZ8" s="3"/>
-      <c r="BA8" s="3"/>
-      <c r="BC8" s="5"/>
-      <c r="BF8" s="5"/>
-      <c r="BJ8" s="5"/>
-      <c r="BL8" s="5"/>
-      <c r="BN8" s="5"/>
-      <c r="BP8" s="5"/>
-      <c r="BZ8" s="5"/>
-      <c r="CB8" s="8"/>
-      <c r="CC8" s="8"/>
-      <c r="CD8" s="8"/>
-      <c r="CE8" s="8"/>
-      <c r="CF8" s="8"/>
-      <c r="CG8" s="8"/>
-      <c r="CH8" s="8"/>
-      <c r="CI8" s="8"/>
-      <c r="CJ8" s="8"/>
-      <c r="CK8" s="8"/>
-      <c r="CL8" s="8"/>
-      <c r="CM8" s="8"/>
-      <c r="CN8" s="8"/>
-      <c r="CO8" s="8"/>
-      <c r="CP8" s="8"/>
-      <c r="CQ8" s="8"/>
-    </row>
-    <row r="11" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="W11" s="5"/>
-      <c r="AP11" s="5"/>
-      <c r="AR11" s="5"/>
-      <c r="AZ11" s="3"/>
-      <c r="BA11" s="3"/>
-      <c r="BC11" s="5"/>
-      <c r="BF11" s="5"/>
-      <c r="BJ11" s="5"/>
-      <c r="BL11" s="5"/>
-      <c r="BN11" s="5"/>
-      <c r="BP11" s="5"/>
-      <c r="BZ11" s="5"/>
-      <c r="CB11" s="8"/>
-      <c r="CC11" s="8"/>
-      <c r="CD11" s="8"/>
-      <c r="CE11" s="8"/>
-      <c r="CF11" s="8"/>
-      <c r="CG11" s="8"/>
-      <c r="CH11" s="8"/>
-      <c r="CI11" s="8"/>
-      <c r="CJ11" s="8"/>
-      <c r="CK11" s="8"/>
-      <c r="CL11" s="8"/>
-      <c r="CM11" s="8"/>
-      <c r="CN11" s="8"/>
-      <c r="CO11" s="8"/>
-      <c r="CP11" s="8"/>
-      <c r="CQ11" s="8"/>
-    </row>
-    <row r="12" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="W12" s="5"/>
-      <c r="AP12" s="5"/>
-      <c r="AR12" s="5"/>
-      <c r="AZ12" s="3"/>
-      <c r="BA12" s="3"/>
-      <c r="BC12" s="5"/>
-      <c r="BF12" s="5"/>
-      <c r="BJ12" s="5"/>
-      <c r="BL12" s="5"/>
-      <c r="BN12" s="5"/>
-      <c r="BP12" s="5"/>
-      <c r="BZ12" s="5"/>
-      <c r="CB12" s="8"/>
-      <c r="CC12" s="8"/>
-      <c r="CD12" s="8"/>
-      <c r="CE12" s="8"/>
-      <c r="CF12" s="8"/>
-      <c r="CG12" s="8"/>
-      <c r="CH12" s="8"/>
-      <c r="CI12" s="8"/>
-      <c r="CJ12" s="8"/>
-      <c r="CK12" s="8"/>
-      <c r="CL12" s="8"/>
-      <c r="CM12" s="8"/>
-      <c r="CN12" s="8"/>
-      <c r="CO12" s="8"/>
-      <c r="CP12" s="8"/>
-      <c r="CQ12" s="8"/>
-    </row>
-    <row r="13" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="W13" s="5"/>
-      <c r="AP13" s="5"/>
-      <c r="AR13" s="5"/>
-      <c r="AZ13" s="3"/>
-      <c r="BA13" s="3"/>
-      <c r="BC13" s="5"/>
-      <c r="BF13" s="5"/>
-      <c r="BJ13" s="5"/>
-      <c r="BL13" s="5"/>
-      <c r="BN13" s="5"/>
-      <c r="BP13" s="5"/>
-      <c r="BZ13" s="5"/>
-      <c r="CB13" s="8"/>
-      <c r="CC13" s="8"/>
-      <c r="CD13" s="8"/>
-      <c r="CE13" s="8"/>
-      <c r="CF13" s="8"/>
-      <c r="CG13" s="8"/>
-      <c r="CH13" s="8"/>
-      <c r="CI13" s="8"/>
-      <c r="CJ13" s="8"/>
-      <c r="CK13" s="8"/>
-      <c r="CL13" s="8"/>
-      <c r="CM13" s="8"/>
-      <c r="CN13" s="8"/>
-      <c r="CO13" s="8"/>
-      <c r="CP13" s="8"/>
-      <c r="CQ13" s="8"/>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0.97950960200000003</v>
+      </c>
+      <c r="AP11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>153</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>156</v>
+      </c>
+      <c r="BE11" t="s">
+        <v>157</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>158</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>159</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>160</v>
+      </c>
+      <c r="BJ11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>161</v>
+      </c>
+      <c r="BL11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>162</v>
+      </c>
+      <c r="BN11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO11" t="s">
+        <v>95</v>
+      </c>
+      <c r="BP11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ11" t="s">
+        <v>163</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>164</v>
+      </c>
+      <c r="BS11" t="s">
+        <v>165</v>
+      </c>
+      <c r="BT11" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU11" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV11" t="s">
+        <v>96</v>
+      </c>
+      <c r="CA11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12">
+        <v>2016</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+      <c r="N12">
+        <v>35</v>
+      </c>
+      <c r="O12">
+        <v>352</v>
+      </c>
+      <c r="P12">
+        <v>55.223333330000003</v>
+      </c>
+      <c r="Q12">
+        <v>15.593666669999999</v>
+      </c>
+      <c r="R12">
+        <v>18.21</v>
+      </c>
+      <c r="S12">
+        <v>6.8</v>
+      </c>
+      <c r="T12">
+        <v>1.96</v>
+      </c>
+      <c r="U12">
+        <v>89</v>
+      </c>
+      <c r="V12">
+        <v>0.74829999999999997</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0.82099125399999995</v>
+      </c>
+      <c r="AP12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>170</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>171</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>172</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>173</v>
+      </c>
+      <c r="BE12" t="s">
+        <v>174</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>175</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>176</v>
+      </c>
+      <c r="BJ12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>177</v>
+      </c>
+      <c r="BL12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>178</v>
+      </c>
+      <c r="BN12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO12" t="s">
+        <v>179</v>
+      </c>
+      <c r="BP12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ12" t="s">
+        <v>180</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>181</v>
+      </c>
+      <c r="BS12" t="s">
+        <v>182</v>
+      </c>
+      <c r="BT12" t="s">
+        <v>183</v>
+      </c>
+      <c r="BU12" t="s">
+        <v>184</v>
+      </c>
+      <c r="BV12" t="s">
+        <v>96</v>
+      </c>
+      <c r="BW12" t="s">
+        <v>185</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13">
+        <v>2016</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>85</v>
+      </c>
+      <c r="N13">
+        <v>40</v>
+      </c>
+      <c r="O13">
+        <v>623</v>
+      </c>
+      <c r="P13">
+        <v>55.223333330000003</v>
+      </c>
+      <c r="Q13">
+        <v>15.593666669999999</v>
+      </c>
+      <c r="R13">
+        <v>18.21</v>
+      </c>
+      <c r="S13">
+        <v>6.8</v>
+      </c>
+      <c r="T13">
+        <v>1.96</v>
+      </c>
+      <c r="U13">
+        <v>89</v>
+      </c>
+      <c r="V13">
+        <v>8.9644999999999992</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0.97343749999999996</v>
+      </c>
+      <c r="AP13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>190</v>
+      </c>
+      <c r="BC13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>191</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>194</v>
+      </c>
+      <c r="BJ13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>195</v>
+      </c>
+      <c r="BL13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>196</v>
+      </c>
+      <c r="BN13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BO13" t="s">
+        <v>95</v>
+      </c>
+      <c r="BP13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>197</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>198</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>199</v>
+      </c>
+      <c r="BT13" t="s">
+        <v>200</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BV13" t="s">
+        <v>96</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="14" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="W14" s="5"/>

</xml_diff>